<commit_message>
Small Changes to Enclosure. Generated STL files for printing
Added extra fastening points, and generated STL files to print printing. Some parts have arrived and others in transit, along with PCB. Should have everything needed to construct a physical device by Wedensday.
</commit_message>
<xml_diff>
--- a/BOM/Bill of Materials.xlsx
+++ b/BOM/Bill of Materials.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="75" documentId="8_{CF17832D-2084-4C23-9887-8E330DC69C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B773630-8A5B-4A4B-8F77-56343F9110BA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{FE1CEC7A-1AA6-4309-9319-B030263357B7}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{FE1CEC7A-1AA6-4309-9319-B030263357B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,10 +498,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791F0209-6CDD-4D83-8499-66BD1B1DD24E}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,17 +859,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1075,17 +1075,17 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1465,17 +1465,17 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -1652,17 +1652,17 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -1810,17 +1810,17 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -1913,17 +1913,17 @@
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
@@ -1970,7 +1970,7 @@
       <c r="E47">
         <v>1</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="7">
         <v>14.2</v>
       </c>
       <c r="G47" t="s">
@@ -1999,7 +1999,7 @@
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F48" s="7">
         <v>15.6</v>
       </c>
       <c r="G48" t="s">

</xml_diff>

<commit_message>
Refactored. Everything implemented except for DFplayer and OLED display
</commit_message>
<xml_diff>
--- a/BOM/Bill of Materials.xlsx
+++ b/BOM/Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3925e46b607fc94d/Documents/PITT/ECE 1895/ECE 1895 Project 2/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{CF17832D-2084-4C23-9887-8E330DC69C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B773630-8A5B-4A4B-8F77-56343F9110BA}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{CF17832D-2084-4C23-9887-8E330DC69C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE4FCAA4-5A56-49FD-AE59-FA3D04DB692F}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{FE1CEC7A-1AA6-4309-9319-B030263357B7}"/>
   </bookViews>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791F0209-6CDD-4D83-8499-66BD1B1DD24E}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +923,7 @@
         <v>109</v>
       </c>
       <c r="H3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>7</v>
@@ -1010,7 +1010,7 @@
         <v>109</v>
       </c>
       <c r="H6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>18</v>
@@ -1645,7 +1645,7 @@
         <v>109</v>
       </c>
       <c r="H31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>106</v>
@@ -1716,7 +1716,7 @@
         <v>109</v>
       </c>
       <c r="H35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>27</v>
@@ -1803,7 +1803,7 @@
         <v>109</v>
       </c>
       <c r="H38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>37</v>
@@ -1874,7 +1874,7 @@
         <v>109</v>
       </c>
       <c r="H42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>41</v>
@@ -1903,7 +1903,7 @@
         <v>109</v>
       </c>
       <c r="H43" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>110</v>

</xml_diff>